<commit_message>
commit du 19 novembre
commit du 19 novembre 2024
</commit_message>
<xml_diff>
--- a/data/situation.xlsx
+++ b/data/situation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER MSI\Documents\R Project\FN_Flood_Response\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E655BF-C86C-4A06-A301-8B879FAF2518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E027302-2051-426C-A517-23069C922BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65A1145B-C151-4FEA-BE04-A4916566AA8A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <r>
       <t>No</t>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Beneficiary Targeting</t>
-  </si>
-  <si>
-    <t>Not Start</t>
   </si>
 </sst>
 </file>
@@ -609,7 +606,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +686,7 @@
         <v>24</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K2" s="5"/>
     </row>

</xml_diff>

<commit_message>
commit du 25 novembre
commit du 25 novembre 2024
</commit_message>
<xml_diff>
--- a/data/situation.xlsx
+++ b/data/situation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER MSI\Documents\R Project\FN_Flood_Response\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E027302-2051-426C-A517-23069C922BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2A0396-0C5D-4D1D-881D-0D4E09341DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65A1145B-C151-4FEA-BE04-A4916566AA8A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <r>
       <t>No</t>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Beneficiary Targeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CBT plus In King  </t>
   </si>
 </sst>
 </file>
@@ -606,7 +609,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,13 +677,13 @@
         <v>20000</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="5">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>24</v>
@@ -738,7 +741,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>20</v>
@@ -750,7 +753,7 @@
         <v>25</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" s="5"/>
     </row>
@@ -891,19 +894,19 @@
       <c r="D9" s="3"/>
       <c r="E9" s="1"/>
       <c r="F9" s="4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="5">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>39</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K9" s="5"/>
     </row>
@@ -963,7 +966,7 @@
         <v>40</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K11" s="5"/>
     </row>

</xml_diff>